<commit_message>
adicionando grafico a planilha
</commit_message>
<xml_diff>
--- a/planilha/dados.xlsx
+++ b/planilha/dados.xlsx
@@ -4,10 +4,11 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Grafico" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -19,7 +20,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,13 +28,23 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="18"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00333333"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -48,9 +59,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -125,6 +139,200 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Historico de Cotaçoes</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Dados'!$A$2:$A$908</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Dados'!$B$2:$B$908</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Dados'!$A$2:$A$908</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Dados'!$C$2:$C$908</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Dados'!$A$2:$A$908</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Dados'!$D$2:$D$908</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Data da Cotaçao</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Valor da Cotaçao</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>2</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="12193200" cy="5335200"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14945,4 +15153,35 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Historico de Cotaçoes</t>
+        </is>
+      </c>
+    </row>
+    <row r="2"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:T2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>